<commit_message>
corrected a duplicated product
</commit_message>
<xml_diff>
--- a/products_bpp.xlsx
+++ b/products_bpp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andriani\Desktop\andriani\UCY\Work_CypErc\BillionPricesCyprusScrape\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andriani\Desktop\andriani\UCY\Work_CypErc\Python Notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913EE4A8-564E-4822-BBF7-829F63FD8575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4582452-AAFA-42CF-A08E-6B4DBB3125FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1847" uniqueCount="842">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="842">
   <si>
     <t>item.name</t>
   </si>
@@ -2956,10 +2956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E385"/>
+  <dimension ref="A1:E384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="56" workbookViewId="0">
-      <selection activeCell="A244" sqref="A244"/>
+    <sheetView tabSelected="1" topLeftCell="A250" zoomScale="56" workbookViewId="0">
+      <selection activeCell="A264" sqref="A264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7444,13 +7444,13 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B264" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="C264" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D264" t="s">
         <v>803</v>
@@ -7461,10 +7461,10 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B265" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="C265" t="s">
         <v>424</v>
@@ -7478,13 +7478,13 @@
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>525</v>
+        <v>823</v>
       </c>
       <c r="B266" t="s">
-        <v>526</v>
+        <v>824</v>
       </c>
       <c r="C266" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D266" t="s">
         <v>803</v>
@@ -7495,10 +7495,10 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>823</v>
+        <v>528</v>
       </c>
       <c r="B267" t="s">
-        <v>824</v>
+        <v>527</v>
       </c>
       <c r="C267" t="s">
         <v>425</v>
@@ -7512,10 +7512,10 @@
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B268" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="C268" t="s">
         <v>425</v>
@@ -7529,10 +7529,10 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="B269" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C269" t="s">
         <v>425</v>
@@ -7546,10 +7546,10 @@
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B270" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="C270" t="s">
         <v>425</v>
@@ -7563,13 +7563,13 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="B271" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="C271" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D271" t="s">
         <v>803</v>
@@ -7580,13 +7580,13 @@
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="B272" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="C272" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D272" t="s">
         <v>803</v>
@@ -7597,10 +7597,10 @@
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B273" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C273" t="s">
         <v>427</v>
@@ -7614,13 +7614,13 @@
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>539</v>
+        <v>833</v>
       </c>
       <c r="B274" t="s">
-        <v>540</v>
+        <v>832</v>
       </c>
       <c r="C274" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D274" t="s">
         <v>803</v>
@@ -7631,10 +7631,10 @@
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>833</v>
+        <v>541</v>
       </c>
       <c r="B275" t="s">
-        <v>832</v>
+        <v>542</v>
       </c>
       <c r="C275" t="s">
         <v>428</v>
@@ -7648,13 +7648,13 @@
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="B276" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="C276" t="s">
-        <v>428</v>
+        <v>457</v>
       </c>
       <c r="D276" t="s">
         <v>803</v>
@@ -7665,10 +7665,10 @@
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="B277" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C277" t="s">
         <v>457</v>
@@ -7682,27 +7682,27 @@
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>546</v>
+        <v>565</v>
       </c>
       <c r="B278" t="s">
-        <v>545</v>
+        <v>557</v>
       </c>
       <c r="C278" t="s">
-        <v>457</v>
+        <v>553</v>
       </c>
       <c r="D278" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="E278" t="s">
-        <v>516</v>
+        <v>552</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B279" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C279" t="s">
         <v>553</v>
@@ -7716,13 +7716,13 @@
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B280" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C280" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D280" t="s">
         <v>804</v>
@@ -7733,10 +7733,10 @@
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B281" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C281" t="s">
         <v>554</v>
@@ -7750,10 +7750,10 @@
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B282" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C282" t="s">
         <v>554</v>
@@ -7767,10 +7767,10 @@
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B283" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C283" t="s">
         <v>554</v>
@@ -7784,13 +7784,13 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B284" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C284" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D284" t="s">
         <v>804</v>
@@ -7801,13 +7801,13 @@
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B285" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C285" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D285" t="s">
         <v>804</v>
@@ -7818,27 +7818,27 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="B286" t="s">
-        <v>564</v>
+        <v>590</v>
       </c>
       <c r="C286" t="s">
-        <v>556</v>
+        <v>574</v>
       </c>
       <c r="D286" t="s">
         <v>804</v>
       </c>
       <c r="E286" t="s">
-        <v>552</v>
+        <v>573</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B287" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C287" t="s">
         <v>574</v>
@@ -7852,13 +7852,13 @@
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B288" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C288" t="s">
-        <v>574</v>
+        <v>554</v>
       </c>
       <c r="D288" t="s">
         <v>804</v>
@@ -7869,10 +7869,10 @@
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B289" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C289" t="s">
         <v>554</v>
@@ -7886,13 +7886,13 @@
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B290" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C290" t="s">
-        <v>554</v>
+        <v>575</v>
       </c>
       <c r="D290" t="s">
         <v>804</v>
@@ -7903,10 +7903,10 @@
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B291" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="C291" t="s">
         <v>575</v>
@@ -7920,10 +7920,10 @@
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B292" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C292" t="s">
         <v>575</v>
@@ -7937,10 +7937,10 @@
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B293" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
       <c r="C293" t="s">
         <v>575</v>
@@ -7954,10 +7954,10 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B294" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="C294" t="s">
         <v>575</v>
@@ -7971,10 +7971,10 @@
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B295" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C295" t="s">
         <v>575</v>
@@ -7988,13 +7988,13 @@
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B296" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="C296" t="s">
-        <v>575</v>
+        <v>555</v>
       </c>
       <c r="D296" t="s">
         <v>804</v>
@@ -8005,10 +8005,10 @@
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B297" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C297" t="s">
         <v>555</v>
@@ -8022,10 +8022,10 @@
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B298" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="C298" t="s">
         <v>555</v>
@@ -8039,13 +8039,13 @@
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B299" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="C299" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D299" t="s">
         <v>804</v>
@@ -8056,27 +8056,27 @@
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
-        <v>589</v>
+        <v>628</v>
       </c>
       <c r="B300" t="s">
-        <v>603</v>
+        <v>678</v>
       </c>
       <c r="C300" t="s">
-        <v>556</v>
+        <v>605</v>
       </c>
       <c r="D300" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E300" t="s">
-        <v>573</v>
+        <v>604</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B301" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="C301" t="s">
         <v>605</v>
@@ -8090,10 +8090,10 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B302" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="C302" t="s">
         <v>605</v>
@@ -8107,13 +8107,13 @@
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B303" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C303" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D303" t="s">
         <v>805</v>
@@ -8124,10 +8124,10 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B304" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="C304" t="s">
         <v>606</v>
@@ -8141,13 +8141,13 @@
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B305" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="C305" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="D305" t="s">
         <v>805</v>
@@ -8158,10 +8158,10 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B306" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="C306" t="s">
         <v>607</v>
@@ -8175,13 +8175,13 @@
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B307" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="C307" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="D307" t="s">
         <v>805</v>
@@ -8192,13 +8192,13 @@
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B308" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="C308" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="D308" t="s">
         <v>805</v>
@@ -8209,13 +8209,13 @@
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B309" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="C309" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D309" t="s">
         <v>805</v>
@@ -8226,13 +8226,13 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B310" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="C310" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D310" t="s">
         <v>805</v>
@@ -8243,10 +8243,10 @@
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B311" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="C311" t="s">
         <v>611</v>
@@ -8260,10 +8260,10 @@
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B312" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="C312" t="s">
         <v>611</v>
@@ -8277,10 +8277,10 @@
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B313" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="C313" t="s">
         <v>611</v>
@@ -8294,13 +8294,13 @@
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B314" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="C314" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D314" t="s">
         <v>805</v>
@@ -8311,13 +8311,13 @@
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B315" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="C315" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="D315" t="s">
         <v>805</v>
@@ -8328,10 +8328,10 @@
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B316" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="C316" t="s">
         <v>613</v>
@@ -8345,16 +8345,16 @@
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B317" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="C317" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D317" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E317" t="s">
         <v>604</v>
@@ -8362,10 +8362,10 @@
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B318" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C318" t="s">
         <v>614</v>
@@ -8379,10 +8379,10 @@
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B319" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="C319" t="s">
         <v>614</v>
@@ -8396,16 +8396,16 @@
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B320" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="C320" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="D320" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="E320" t="s">
         <v>604</v>
@@ -8413,13 +8413,13 @@
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B321" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="C321" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D321" t="s">
         <v>807</v>
@@ -8430,10 +8430,10 @@
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B322" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="C322" t="s">
         <v>616</v>
@@ -8447,13 +8447,13 @@
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B323" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="C323" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D323" t="s">
         <v>807</v>
@@ -8464,13 +8464,13 @@
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B324" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="C324" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D324" t="s">
         <v>807</v>
@@ -8481,13 +8481,13 @@
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B325" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="C325" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D325" t="s">
         <v>807</v>
@@ -8498,10 +8498,10 @@
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B326" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="C326" t="s">
         <v>619</v>
@@ -8515,10 +8515,10 @@
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B327" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="C327" t="s">
         <v>619</v>
@@ -8532,13 +8532,13 @@
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B328" t="s">
-        <v>705</v>
+        <v>717</v>
       </c>
       <c r="C328" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D328" t="s">
         <v>807</v>
@@ -8549,13 +8549,13 @@
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B329" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="C329" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D329" t="s">
         <v>807</v>
@@ -8566,13 +8566,13 @@
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B330" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C330" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D330" t="s">
         <v>807</v>
@@ -8583,13 +8583,13 @@
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B331" t="s">
-        <v>719</v>
+        <v>706</v>
       </c>
       <c r="C331" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D331" t="s">
         <v>807</v>
@@ -8600,13 +8600,13 @@
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B332" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="C332" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D332" t="s">
         <v>807</v>
@@ -8617,13 +8617,13 @@
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B333" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="C333" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D333" t="s">
         <v>807</v>
@@ -8634,16 +8634,16 @@
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B334" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C334" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D334" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="E334" t="s">
         <v>604</v>
@@ -8651,10 +8651,10 @@
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B335" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C335" t="s">
         <v>626</v>
@@ -8668,10 +8668,10 @@
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B336" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="C336" t="s">
         <v>626</v>
@@ -8685,10 +8685,10 @@
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B337" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C337" t="s">
         <v>626</v>
@@ -8702,13 +8702,13 @@
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
-        <v>665</v>
+        <v>715</v>
       </c>
       <c r="B338" t="s">
-        <v>712</v>
-      </c>
-      <c r="C338" t="s">
-        <v>626</v>
+        <v>714</v>
+      </c>
+      <c r="C338" s="3" t="s">
+        <v>716</v>
       </c>
       <c r="D338" t="s">
         <v>808</v>
@@ -8719,13 +8719,13 @@
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
-        <v>715</v>
+        <v>666</v>
       </c>
       <c r="B339" t="s">
-        <v>714</v>
-      </c>
-      <c r="C339" s="3" t="s">
-        <v>716</v>
+        <v>713</v>
+      </c>
+      <c r="C339" t="s">
+        <v>627</v>
       </c>
       <c r="D339" t="s">
         <v>808</v>
@@ -8736,27 +8736,27 @@
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
-        <v>666</v>
+        <v>746</v>
       </c>
       <c r="B340" t="s">
-        <v>713</v>
+        <v>720</v>
       </c>
       <c r="C340" t="s">
-        <v>627</v>
+        <v>668</v>
       </c>
       <c r="D340" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="E340" t="s">
-        <v>604</v>
+        <v>667</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="B341" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C341" t="s">
         <v>668</v>
@@ -8770,13 +8770,13 @@
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B342" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C342" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D342" t="s">
         <v>805</v>
@@ -8787,10 +8787,10 @@
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B343" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="C343" t="s">
         <v>669</v>
@@ -8804,13 +8804,13 @@
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B344" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C344" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="D344" t="s">
         <v>805</v>
@@ -8821,10 +8821,10 @@
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B345" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C345" t="s">
         <v>670</v>
@@ -8838,10 +8838,10 @@
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B346" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="C346" t="s">
         <v>670</v>
@@ -8855,10 +8855,10 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B347" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="C347" t="s">
         <v>670</v>
@@ -8872,10 +8872,10 @@
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B348" t="s">
-        <v>727</v>
+        <v>825</v>
       </c>
       <c r="C348" t="s">
         <v>670</v>
@@ -8889,10 +8889,10 @@
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B349" t="s">
-        <v>825</v>
+        <v>728</v>
       </c>
       <c r="C349" t="s">
         <v>670</v>
@@ -8906,13 +8906,13 @@
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B350" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C350" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D350" t="s">
         <v>805</v>
@@ -8923,10 +8923,10 @@
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B351" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="C351" t="s">
         <v>671</v>
@@ -8940,10 +8940,10 @@
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B352" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C352" t="s">
         <v>671</v>
@@ -8957,13 +8957,13 @@
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B353" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C353" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D353" t="s">
         <v>805</v>
@@ -8974,10 +8974,10 @@
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B354" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C354" t="s">
         <v>672</v>
@@ -8991,10 +8991,10 @@
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B355" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="C355" t="s">
         <v>672</v>
@@ -9008,13 +9008,13 @@
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B356" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="C356" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D356" t="s">
         <v>805</v>
@@ -9025,10 +9025,10 @@
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B357" t="s">
-        <v>735</v>
+        <v>835</v>
       </c>
       <c r="C357" t="s">
         <v>673</v>
@@ -9042,16 +9042,16 @@
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B358" t="s">
-        <v>835</v>
+        <v>736</v>
       </c>
       <c r="C358" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="D358" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="E358" t="s">
         <v>667</v>
@@ -9059,10 +9059,10 @@
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B359" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C359" t="s">
         <v>674</v>
@@ -9076,10 +9076,10 @@
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B360" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="C360" t="s">
         <v>674</v>
@@ -9093,13 +9093,13 @@
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B361" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="C361" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="D361" t="s">
         <v>807</v>
@@ -9110,10 +9110,10 @@
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B362" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C362" t="s">
         <v>675</v>
@@ -9127,10 +9127,10 @@
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B363" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C363" t="s">
         <v>675</v>
@@ -9144,13 +9144,13 @@
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B364" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="C364" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="D364" t="s">
         <v>807</v>
@@ -9161,10 +9161,10 @@
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>770</v>
+        <v>834</v>
       </c>
       <c r="B365" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C365" t="s">
         <v>676</v>
@@ -9178,13 +9178,13 @@
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>834</v>
+        <v>771</v>
       </c>
       <c r="B366" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="C366" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="D366" t="s">
         <v>807</v>
@@ -9195,10 +9195,10 @@
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B367" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="C367" t="s">
         <v>677</v>
@@ -9212,10 +9212,10 @@
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>772</v>
+        <v>837</v>
       </c>
       <c r="B368" t="s">
-        <v>740</v>
+        <v>836</v>
       </c>
       <c r="C368" t="s">
         <v>677</v>
@@ -9227,16 +9227,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A369" t="s">
-        <v>837</v>
-      </c>
-      <c r="B369" t="s">
-        <v>836</v>
-      </c>
-      <c r="C369" t="s">
-        <v>677</v>
-      </c>
+    <row r="369" spans="2:5" x14ac:dyDescent="0.35">
       <c r="D369" t="s">
         <v>807</v>
       </c>
@@ -9244,49 +9235,41 @@
         <v>667</v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D370" t="s">
-        <v>807</v>
-      </c>
-      <c r="E370" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="373" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B373" s="4"/>
+    </row>
+    <row r="374" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B374" s="4"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="375" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B375" s="4"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="376" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B376" s="4"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="377" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B377" s="4"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="378" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B378" s="4"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="379" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B379" s="4"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="380" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B380" s="4"/>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="381" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B381" s="4"/>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="382" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B382" s="4"/>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="383" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B383" s="4"/>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="384" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B384" s="4"/>
-    </row>
-    <row r="385" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B385" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
famous sport product name changed
</commit_message>
<xml_diff>
--- a/products_bpp.xlsx
+++ b/products_bpp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andriani\Desktop\andriani\UCY\Work_CypErc\BillionPricesCyprusScrape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C1CC75-1E2E-4F89-81EC-507564288493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F253DE-1062-4A45-9AA1-0DC3F3A21B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="842">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="843">
   <si>
     <t>item.name</t>
   </si>
@@ -2560,6 +2560,9 @@
   </si>
   <si>
     <t>adidas men future icons 3-stripes shorts (IC3752)</t>
+  </si>
+  <si>
+    <t>adidas women adidas sportswear future icons winners 3.0 t-sh</t>
   </si>
 </sst>
 </file>
@@ -2958,8 +2961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A349" zoomScale="56" workbookViewId="0">
-      <selection activeCell="D369" sqref="D369"/>
+    <sheetView tabSelected="1" topLeftCell="A229" zoomScale="56" workbookViewId="0">
+      <selection activeCell="A249" sqref="A249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7189,7 +7192,7 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>491</v>
+        <v>842</v>
       </c>
       <c r="B249" t="s">
         <v>492</v>

</xml_diff>